<commit_message>
new commit related to excel data read
</commit_message>
<xml_diff>
--- a/src/test/resources/excelsheets/TestData.xlsx
+++ b/src/test/resources/excelsheets/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Cucumbe_-Karate_RestAssurred_API_Automation\SeleniumJavaAutomation_NewSite\src\test\resources\excelsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0C2A54F-2A5D-444E-9084-4FB29633C031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F1AF74-2B5B-469A-97D8-CDE38BE45CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A144C4B7-8703-4116-8F39-8F22B673AD23}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{A144C4B7-8703-4116-8F39-8F22B673AD23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,14 +70,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,17 +98,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,7 +421,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,7 +438,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -467,8 +456,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E4236ABA-CA43-40D1-BFE0-1C97318D64B9}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1F6E2539-5B35-4228-A0F0-9DC789EE6C18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new commit 27th Feb
</commit_message>
<xml_diff>
--- a/src/test/resources/excelsheets/TestData.xlsx
+++ b/src/test/resources/excelsheets/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Cucumbe_-Karate_RestAssurred_API_Automation\SeleniumJavaAutomation_NewSite\src\test\resources\excelsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d9ad9314d52015b/Desktop/New folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F1AF74-2B5B-469A-97D8-CDE38BE45CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{663BF080-AE5F-4B7A-8F4F-206C6488FF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14F6DD05-8774-4882-AE44-F9B9226D4F28}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{A144C4B7-8703-4116-8F39-8F22B673AD23}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C84C77DA-10D7-4E8E-BD45-CDA21B6B6942}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -417,11 +419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2CE217-4F6E-4B26-BB4C-BC8548D43023}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CE4B63-B737-4436-AA8B-31521F881FC6}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,10 +457,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{E4236ABA-CA43-40D1-BFE0-1C97318D64B9}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{1F6E2539-5B35-4228-A0F0-9DC789EE6C18}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8D9BE3AB-C62B-461E-9580-ED9B27F42706}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{82DBC106-B9CF-4EE3-94CE-6BC208651310}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>